<commit_message>
checking status of fake_data_complete and pushing some intermediate changes
</commit_message>
<xml_diff>
--- a/ref/preliminary_calibration_info/afolu_fao_calibration_by_subsector.xlsx
+++ b/ref/preliminary_calibration_info/afolu_fao_calibration_by_subsector.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsyme/Documents/Projects/git_jbus/lac_decarbonization/ref/preliminary_calibration_info/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{32E0007A-52F6-5C4F-9A1E-CD57A02B8F27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{0E8B901E-F3F2-BD46-8E7B-492D85F2347A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13980" yWindow="11080" windowWidth="26840" windowHeight="15940"/>
+    <workbookView xWindow="1500" yWindow="1800" windowWidth="26840" windowHeight="15940"/>
   </bookViews>
   <sheets>
     <sheet name="afolu_fao_calibration_by_subsec" sheetId="1" r:id="rId1"/>
@@ -1381,8 +1381,8 @@
   <dimension ref="A1:BR26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="7" topLeftCell="AY1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BA2" sqref="BA2"/>
+      <pane xSplit="7" topLeftCell="AR1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="BB2" sqref="BB2:BD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
updated calibration crosswalk for FAO data
</commit_message>
<xml_diff>
--- a/ref/preliminary_calibration_info/afolu_fao_calibration_by_subsector.xlsx
+++ b/ref/preliminary_calibration_info/afolu_fao_calibration_by_subsector.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsyme/Documents/Projects/git_jbus/lac_decarbonization/ref/preliminary_calibration_info/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9B8BB4F-289E-B24F-9BE9-E2C3016A7330}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA6A3E66-7DD4-E34C-9D21-C8DBD7952498}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="1800" windowWidth="34340" windowHeight="19260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="540" yWindow="460" windowWidth="34340" windowHeight="19260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="afolu_fao_calibration_by_subsec" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="116">
   <si>
     <t>Item Code</t>
   </si>
@@ -377,6 +377,9 @@
   </si>
   <si>
     <t>NOT AVAILABLE IN FAO ACCOUNTING</t>
+  </si>
+  <si>
+    <t>DATASET: Emissions_Totals_E_All_Data_(Normalized)</t>
   </si>
 </sst>
 </file>
@@ -1487,11 +1490,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BR27"/>
+  <dimension ref="A1:BR28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="7" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J23" sqref="J23"/>
+      <pane xSplit="7" topLeftCell="L1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3848,6 +3851,11 @@
         <v>-8.7311491370201111E-11</v>
       </c>
     </row>
+    <row r="28" spans="1:70" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>115</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="14">
     <mergeCell ref="BB1:BR1"/>

</xml_diff>